<commit_message>
Changed plume identification guidence
Now plume with a diffraction spike is noted as not being a CH4 emission owing to that it is more likely water and C02 in the signal not methane
</commit_message>
<xml_diff>
--- a/Data/Plume_training_master.xlsx
+++ b/Data/Plume_training_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIS_Course\Methane_Point_Detection\Sentinel-2_Algeria_Methane\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7D7CEC-D602-4C7C-9D13-6B31FCD7EECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BD1AD2-8FC9-4EE0-A34B-3BD0E030EF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{74612387-FD74-4A34-93E0-277F276CE390}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{74612387-FD74-4A34-93E0-277F276CE390}"/>
   </bookViews>
   <sheets>
     <sheet name="Plume Training" sheetId="6" r:id="rId1"/>
@@ -335,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -359,12 +359,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,7 +910,7 @@
               <c:f>'Plume Training'!$J$2:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>5.4530000000000003</c:v>
                 </c:pt>
@@ -927,27 +921,45 @@
                   <c:v>8.4969999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>4.3259999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7570000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
                   <c:v>3.6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11">
                   <c:v>4.8</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13">
                   <c:v>2.7</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14">
                   <c:v>2.1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="15">
                   <c:v>14.8</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -958,7 +970,7 @@
               <c:f>'Plume Training'!$L$2:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>5.3848799999999999</c:v>
                 </c:pt>
@@ -969,21 +981,39 @@
                   <c:v>5.2594200000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.779579999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2.6886300000000003</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
                   <c:v>2.0910900000000003</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11">
                   <c:v>2.3590500000000003</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
                   <c:v>3.27014</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="15">
                   <c:v>10.53646</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1305,10 +1335,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="108"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="8"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1329,9 +1359,26 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Study Q vs IME Q </a:t>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Q</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>IME </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>vs Study Q </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1357,7 +1404,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1393,11 +1440,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1422,7 +1469,7 @@
             </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:ln w="25400" cap="rnd">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -1564,7 +1611,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -1574,7 +1621,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1050"/>
                   <a:t>Study Q t/h</a:t>
                 </a:r>
               </a:p>
@@ -1593,7 +1640,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -1673,7 +1720,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -1683,8 +1730,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>CSF Q t/h</a:t>
+                  <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Q</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>IME</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t> t/h</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1702,7 +1761,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -1816,14 +1875,78 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="108"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="8"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Q</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="-25000">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>M </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>vs Q</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="-25000">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>IME </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1837,7 +1960,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1882,11 +2005,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2137,7 +2260,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -2147,8 +2270,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>QIME t/h</a:t>
+                  <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Q</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>IME</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t> t/h</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2166,7 +2301,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -2246,7 +2381,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -2256,8 +2391,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>QM t/h</a:t>
+                  <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Q</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>M</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t> t/h</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2275,7 +2422,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -2423,82 +2570,14 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="26">
   <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="26">
   <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -4097,14 +4176,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>296956</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>158002</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>131885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>67234</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>32496</xdr:rowOff>
+      <xdr:rowOff>32497</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4132,15 +4211,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>281421</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>82262</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>58615</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>545523</xdr:colOff>
+      <xdr:colOff>542192</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>12988</xdr:rowOff>
+      <xdr:rowOff>14654</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4155,15 +4234,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3290455" y="4030807"/>
-          <a:ext cx="2424545" cy="1749136"/>
+          <a:off x="3304442" y="3773365"/>
+          <a:ext cx="2417885" cy="1970943"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="12700">
           <a:solidFill>
-            <a:srgbClr val="FF0000"/>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="dash"/>
         </a:ln>
@@ -4229,15 +4310,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>164523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:colOff>294409</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>103909</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4252,16 +4333,19 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4152900" y="1914525"/>
-          <a:ext cx="2981325" cy="2552700"/>
+          <a:off x="4182341" y="1982932"/>
+          <a:ext cx="2935432" cy="2485159"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="FF0000"/>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
           </a:solidFill>
+          <a:prstDash val="dash"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -4732,8 +4816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49870DD-AD43-4575-B0E6-4E5738AF0BC2}">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView topLeftCell="M11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5059,7 +5143,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="21" hidden="1" customHeight="1">
+    <row r="5" spans="1:23" ht="21" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5133,7 +5217,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="21" hidden="1" customHeight="1">
+    <row r="6" spans="1:23" ht="21" customHeight="1">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5207,7 +5291,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="21" hidden="1" customHeight="1">
+    <row r="7" spans="1:23" ht="21" customHeight="1">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5281,7 +5365,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="21" hidden="1" customHeight="1">
+    <row r="8" spans="1:23" ht="21" customHeight="1">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5358,7 +5442,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="21" hidden="1" customHeight="1">
+    <row r="9" spans="1:23" ht="21" customHeight="1">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5432,7 +5516,7 @@
         <v>0.49480324074074072</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="21" hidden="1" customHeight="1">
+    <row r="10" spans="1:23" ht="21" customHeight="1">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6084,8 +6168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A352D59B-51B3-410D-89FA-36B5827EC7D6}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7580,8 +7664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7873113-BB9E-42AB-91B4-21E5DEE28100}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8093,7 +8177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9044E-A1C0-41D1-A275-514B5A2368CC}">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A78" sqref="A78:XFD78"/>
     </sheetView>
   </sheetViews>
@@ -11596,48 +11680,48 @@
         <v>5.56</v>
       </c>
     </row>
-    <row r="78" spans="1:14" s="13" customFormat="1">
-      <c r="A78" s="13">
+    <row r="78" spans="1:14">
+      <c r="A78">
         <v>69</v>
       </c>
-      <c r="B78" s="14">
+      <c r="B78" s="5">
         <v>44059</v>
       </c>
-      <c r="C78" s="14">
+      <c r="C78" s="5">
         <v>43947</v>
       </c>
-      <c r="D78" s="13">
+      <c r="D78">
         <v>31.7773</v>
       </c>
-      <c r="E78" s="13">
+      <c r="E78">
         <v>5.9941000000000004</v>
       </c>
-      <c r="F78" s="15">
+      <c r="F78" s="1">
         <v>10370.629999999999</v>
       </c>
-      <c r="G78" s="15">
+      <c r="G78" s="1">
         <v>17720.060000000001</v>
       </c>
-      <c r="H78" s="16">
+      <c r="H78" s="11">
         <f t="shared" si="2"/>
         <v>17.72006</v>
       </c>
-      <c r="I78" s="13">
+      <c r="I78">
         <v>25.8935222625732</v>
       </c>
-      <c r="J78" s="15">
+      <c r="J78" s="1">
         <v>11</v>
       </c>
-      <c r="K78" s="17">
+      <c r="K78" s="4">
         <v>0.12865199999999999</v>
       </c>
-      <c r="L78" s="18">
+      <c r="L78" s="3">
         <v>22.561028</v>
       </c>
-      <c r="M78" s="13">
+      <c r="M78">
         <v>1.8602609999999999</v>
       </c>
-      <c r="N78" s="13">
+      <c r="N78">
         <v>5.19</v>
       </c>
     </row>
@@ -12641,7 +12725,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E23" sqref="E22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Named the software CH4 Sentinel and adjusted documentation accordingly.
</commit_message>
<xml_diff>
--- a/Data/Plume_training_master.xlsx
+++ b/Data/Plume_training_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIS_Course\Methane_Point_Detection\Sentinel-2_Algeria_Methane\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BD1AD2-8FC9-4EE0-A34B-3BD0E030EF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C936634-F9AC-4797-B986-EA63379ADE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{74612387-FD74-4A34-93E0-277F276CE390}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="2" xr2:uid="{74612387-FD74-4A34-93E0-277F276CE390}"/>
   </bookViews>
   <sheets>
     <sheet name="Plume Training" sheetId="6" r:id="rId1"/>
@@ -4242,9 +4242,7 @@
         </a:prstGeom>
         <a:ln w="12700">
           <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:prstDash val="dash"/>
         </a:ln>
@@ -4341,9 +4339,7 @@
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:prstDash val="dash"/>
         </a:ln>
@@ -6168,8 +6164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A352D59B-51B3-410D-89FA-36B5827EC7D6}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="E18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7664,8 +7660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7873113-BB9E-42AB-91B4-21E5DEE28100}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>